<commit_message>
Accomodate headers with leading and trailing whitespace
To allow processing of files with headers that have spaces
padded, which is a common occurence
</commit_message>
<xml_diff>
--- a/core/src/test/resources/test_people.xlsx
+++ b/core/src/test/resources/test_people.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\projects\zerocell\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikani\Projects\zerocell\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,26 +77,33 @@
     <t>Mpulula</t>
   </si>
   <si>
-    <t>FAV_NUMBER</t>
-  </si>
-  <si>
-    <t>DATE_REGISTERED</t>
-  </si>
-  <si>
-    <t>MIDDLE_NAME</t>
-  </si>
-  <si>
-    <t>LAST_NAME</t>
+    <t xml:space="preserve">LAST_NAME  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   DATE_REGISTERED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAV_NUMBER   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIDDLE_NAME  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,150 +419,153 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>34062</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>40909</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>34475</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>42339</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>32198</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>42675</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>31507</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>42430</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>33613</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>42644</v>
       </c>
     </row>

</xml_diff>